<commit_message>
add packml library and begin working on build errors
</commit_message>
<xml_diff>
--- a/TwinCAT/Documents/Axis Calculations.xlsx
+++ b/TwinCAT/Documents/Axis Calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitHub\ArfBotOS\TwinCAT\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C84D3129-D9D3-42F1-AD16-BDDF4EDF120C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4081AD1-BEED-4ADD-B7E0-F21F934C2D3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="16860" xr2:uid="{BC95E908-8886-4A1F-AE2F-C946640122CC}"/>
+    <workbookView xWindow="6105" yWindow="735" windowWidth="18000" windowHeight="12150" xr2:uid="{BC95E908-8886-4A1F-AE2F-C946640122CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,9 +44,6 @@
     <t>Degrees per revolution</t>
   </si>
   <si>
-    <t>Pullses per Revolution</t>
-  </si>
-  <si>
     <t>M1</t>
   </si>
   <si>
@@ -66,6 +63,9 @@
   </si>
   <si>
     <t>Reference Velocity</t>
+  </si>
+  <si>
+    <t>Pulses per Revolution</t>
   </si>
 </sst>
 </file>
@@ -501,7 +501,7 @@
   <dimension ref="F6:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -520,15 +520,15 @@
         <v>1</v>
       </c>
       <c r="I6" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="K6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G7" s="2">
         <v>32767</v>
@@ -546,7 +546,7 @@
     </row>
     <row r="8" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G8" s="2">
         <v>32767</v>
@@ -564,7 +564,7 @@
     </row>
     <row r="9" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G9" s="2">
         <v>32767</v>
@@ -582,7 +582,7 @@
     </row>
     <row r="10" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G10" s="2">
         <v>32767</v>
@@ -601,7 +601,7 @@
     </row>
     <row r="11" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G11" s="2">
         <v>32767</v>
@@ -620,7 +620,7 @@
     </row>
     <row r="12" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G12" s="2">
         <v>32767</v>

</xml_diff>

<commit_message>
tweak encoder ratios. update spreadsheet.
</commit_message>
<xml_diff>
--- a/TwinCAT/Documents/Axis Calculations.xlsx
+++ b/TwinCAT/Documents/Axis Calculations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitHub\ArfBotOS\TwinCAT\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dalet\Documents\GitHub\ArfBotOS\TwinCAT\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4081AD1-BEED-4ADD-B7E0-F21F934C2D3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEAE5E8D-9D9A-4EFF-97F0-440C23EBE5AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6105" yWindow="735" windowWidth="18000" windowHeight="12150" xr2:uid="{BC95E908-8886-4A1F-AE2F-C946640122CC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="44640" windowHeight="21615" xr2:uid="{BC95E908-8886-4A1F-AE2F-C946640122CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Drive Output Scale</t>
   </si>
@@ -62,16 +62,40 @@
     <t>M6</t>
   </si>
   <si>
-    <t>Reference Velocity</t>
-  </si>
-  <si>
-    <t>Pulses per Revolution</t>
+    <t>Reduction Factor</t>
+  </si>
+  <si>
+    <t>Motor Steps per Revolution</t>
+  </si>
+  <si>
+    <t>Encoder Counts per Revolution</t>
+  </si>
+  <si>
+    <t>Encoder Pulses per User Unit (Degree)</t>
+  </si>
+  <si>
+    <t>Effective Motor Steps per Revolution</t>
+  </si>
+  <si>
+    <t>Encoder Scaling Factor Numerator</t>
+  </si>
+  <si>
+    <t>Drive Reference Velocity</t>
+  </si>
+  <si>
+    <t>Drive</t>
+  </si>
+  <si>
+    <t>Encoder</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="172" formatCode="0.000000000000000000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -90,7 +114,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -114,7 +138,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -138,17 +162,30 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
+      <right/>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -156,17 +193,26 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1"/>
+    <xf numFmtId="172" fontId="2" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
+    <cellStyle name="Calculation" xfId="2" builtinId="22"/>
     <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Output" xfId="2" builtinId="21"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -498,146 +544,299 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AFD2E7A-B27D-4E92-84C9-38B140952E34}">
-  <dimension ref="F6:K12"/>
+  <dimension ref="B5:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" customWidth="1"/>
+    <col min="9" max="9" width="3.140625" customWidth="1"/>
+    <col min="10" max="10" width="16.5703125" customWidth="1"/>
+    <col min="11" max="11" width="17.5703125" customWidth="1"/>
+    <col min="12" max="12" width="23.140625" customWidth="1"/>
+    <col min="13" max="13" width="23" customWidth="1"/>
+    <col min="14" max="14" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="G6" t="s">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="J5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+    </row>
+    <row r="6" spans="2:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H6" t="s">
+      <c r="D6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="I6" t="s">
+      <c r="E6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K6" t="s">
-        <v>8</v>
+      <c r="G6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="7" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F7" t="s">
+    <row r="7" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
         <v>2</v>
       </c>
-      <c r="G7" s="2">
+      <c r="C7" s="1">
         <v>32767</v>
       </c>
-      <c r="H7" s="2">
+      <c r="D7" s="1">
         <v>360</v>
       </c>
-      <c r="I7" s="2">
+      <c r="E7" s="1">
+        <f>(10*4)</f>
+        <v>40</v>
+      </c>
+      <c r="F7" s="1">
+        <v>400</v>
+      </c>
+      <c r="G7" s="4">
+        <f>E7*F7</f>
         <v>16000</v>
       </c>
-      <c r="K7" s="1">
-        <f>(H7/I7)*G7</f>
+      <c r="H7" s="5">
+        <f>(D7/G7)*C7</f>
         <v>737.25749999999994</v>
       </c>
+      <c r="J7" s="1">
+        <v>4000</v>
+      </c>
+      <c r="K7" s="4">
+        <f>(E7*J7)/D7</f>
+        <v>444.44444444444446</v>
+      </c>
+      <c r="L7" s="6">
+        <f>1/K7</f>
+        <v>2.2499999999999998E-3</v>
+      </c>
     </row>
-    <row r="8" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F8" t="s">
+    <row r="8" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
         <v>3</v>
       </c>
-      <c r="G8" s="2">
+      <c r="C8" s="1">
         <v>32767</v>
       </c>
-      <c r="H8" s="2">
+      <c r="D8" s="1">
         <v>360</v>
       </c>
-      <c r="I8" s="2">
+      <c r="E8" s="1">
+        <v>50</v>
+      </c>
+      <c r="F8" s="1">
+        <v>400</v>
+      </c>
+      <c r="G8" s="4">
         <v>20000</v>
       </c>
-      <c r="K8" s="1">
-        <f t="shared" ref="K8:K12" si="0">(H8/I8)*G8</f>
+      <c r="H8" s="5">
+        <f>(D8/G8)*C8</f>
         <v>589.80599999999993</v>
       </c>
+      <c r="J8" s="1">
+        <v>4000</v>
+      </c>
+      <c r="K8" s="4">
+        <f>(E8*J8)/D8</f>
+        <v>555.55555555555554</v>
+      </c>
+      <c r="L8" s="6">
+        <f t="shared" ref="L8:L12" si="0">1/K8</f>
+        <v>1.8E-3</v>
+      </c>
     </row>
-    <row r="9" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F9" t="s">
+    <row r="9" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
         <v>4</v>
       </c>
-      <c r="G9" s="2">
+      <c r="C9" s="1">
         <v>32767</v>
       </c>
-      <c r="H9" s="2">
+      <c r="D9" s="1">
         <v>360</v>
       </c>
-      <c r="I9" s="2">
+      <c r="E9" s="1">
+        <v>50</v>
+      </c>
+      <c r="F9" s="1">
+        <v>400</v>
+      </c>
+      <c r="G9" s="4">
         <v>20000</v>
       </c>
-      <c r="K9" s="1">
+      <c r="H9" s="5">
+        <f>(D9/G9)*C9</f>
+        <v>589.80599999999993</v>
+      </c>
+      <c r="J9" s="1">
+        <v>4000</v>
+      </c>
+      <c r="K9" s="4">
+        <f>(E9*J9)/D9</f>
+        <v>555.55555555555554</v>
+      </c>
+      <c r="L9" s="6">
         <f t="shared" si="0"/>
-        <v>589.80599999999993</v>
+        <v>1.8E-3</v>
       </c>
     </row>
-    <row r="10" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F10" t="s">
+    <row r="10" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
         <v>5</v>
       </c>
-      <c r="G10" s="2">
+      <c r="C10" s="1">
         <v>32767</v>
       </c>
-      <c r="H10" s="2">
+      <c r="D10" s="1">
         <v>360</v>
       </c>
-      <c r="I10" s="2">
-        <f>16*(28/10)*600</f>
+      <c r="E10" s="1">
+        <f>16*(28/10)</f>
+        <v>44.8</v>
+      </c>
+      <c r="F10" s="1">
+        <v>600</v>
+      </c>
+      <c r="G10" s="4">
+        <f>E10*F10</f>
         <v>26880</v>
       </c>
-      <c r="K10" s="1">
+      <c r="H10" s="5">
+        <f>(D10/G10)*C10</f>
+        <v>438.84375</v>
+      </c>
+      <c r="J10" s="1">
+        <v>4000</v>
+      </c>
+      <c r="K10" s="4">
+        <f>(E10*J10)/D10</f>
+        <v>497.77777777777777</v>
+      </c>
+      <c r="L10" s="6">
         <f t="shared" si="0"/>
-        <v>438.84375</v>
+        <v>2.0089285714285717E-3</v>
       </c>
     </row>
-    <row r="11" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F11" t="s">
+    <row r="11" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="2">
+      <c r="C11" s="1">
         <v>32767</v>
       </c>
-      <c r="H11" s="2">
+      <c r="D11" s="1">
         <v>360</v>
       </c>
-      <c r="I11" s="2">
-        <f>((25*3.14)/8)*800</f>
+      <c r="E11" s="1">
+        <f>((25*3.14)/8)</f>
+        <v>9.8125</v>
+      </c>
+      <c r="F11" s="1">
+        <v>800</v>
+      </c>
+      <c r="G11" s="4">
+        <f>E11*F11</f>
         <v>7850</v>
       </c>
-      <c r="K11" s="1">
+      <c r="H11" s="5">
+        <f>(D11/G11)*C11</f>
+        <v>1502.6904458598724</v>
+      </c>
+      <c r="J11" s="1">
+        <v>4000</v>
+      </c>
+      <c r="K11" s="4">
+        <f>(E11*J11)/D11</f>
+        <v>109.02777777777777</v>
+      </c>
+      <c r="L11" s="6">
         <f t="shared" si="0"/>
-        <v>1502.6904458598724</v>
+        <v>9.1719745222929947E-3</v>
       </c>
     </row>
-    <row r="12" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F12" t="s">
+    <row r="12" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
         <v>7</v>
       </c>
-      <c r="G12" s="2">
+      <c r="C12" s="1">
         <v>32767</v>
       </c>
-      <c r="H12" s="2">
+      <c r="D12" s="1">
         <v>360</v>
       </c>
-      <c r="I12" s="2">
-        <f>(1293/64)*400</f>
+      <c r="E12" s="1">
+        <f>(1293/64)</f>
+        <v>20.203125</v>
+      </c>
+      <c r="F12" s="1">
+        <v>400</v>
+      </c>
+      <c r="G12" s="4">
+        <f>E12*F12</f>
         <v>8081.25</v>
       </c>
-      <c r="K12" s="1">
+      <c r="H12" s="5">
+        <f>(D12/G12)*C12</f>
+        <v>1459.6900232018561</v>
+      </c>
+      <c r="J12" s="1">
+        <v>4000</v>
+      </c>
+      <c r="K12" s="4">
+        <f>(E12*J12)/D12</f>
+        <v>224.47916666666666</v>
+      </c>
+      <c r="L12" s="6">
         <f t="shared" si="0"/>
-        <v>1459.6900232018561</v>
-      </c>
+        <v>4.4547563805104407E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="M15" s="2"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="J5:L5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>